<commit_message>
added study 2 data sheet
</commit_message>
<xml_diff>
--- a/study 3 results - revised.xlsx
+++ b/study 3 results - revised.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\online vid proj 2\Online-Vid-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6C2F8A-F727-4B18-A5AF-6AC57B91AC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE7066F-F000-40DA-8BF7-4FFBFFE2CAD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3315" yWindow="7020" windowWidth="13830" windowHeight="7170" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary of Results" sheetId="2" r:id="rId1"/>

</xml_diff>